<commit_message>
Removed details from CMP and added example
</commit_message>
<xml_diff>
--- a/CMP_data.xlsx
+++ b/CMP_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\as255178\DC\CMP python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\as255178\DC\CMP python\Automating-CMP-Details-Generation-with-Python-Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245D72CE-93A6-4833-8E24-C9F62D6F0ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F7BAF5-0620-4D91-9991-DD1C530E9E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,13 +43,13 @@
     <t>Summary</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
     <t>Waiting</t>
   </si>
   <si>
     <t>Task of the ticket</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -972,7 +972,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="5.0999999999999996" x14ac:dyDescent="0.2"/>
@@ -1014,10 +1014,10 @@
     </row>
     <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="9">
         <v>45231.870833333334</v>
@@ -1028,7 +1028,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2" s="10"/>
     </row>
@@ -1043,7 +1043,6 @@
       <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" ht="13.8" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1063,12 +1062,9 @@
       <c r="H5" s="6"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="https://collaboration.msi.audi.com/jira/browse/ADP-7178" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-  </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.5" header="0.5" footer="0.25"/>
-  <pageSetup orientation="landscape" r:id="rId2"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>